<commit_message>
Added Delay total to spreadsheet
</commit_message>
<xml_diff>
--- a/Part 1 Data.xlsx
+++ b/Part 1 Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E38AE6-0B9E-4184-97DC-B5DE55ADDD7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619E9570-F3D0-4E09-AA3E-A63FBA5EFD72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$145</definedName>
     <definedName name="Hackathon_Data_File_2__3" localSheetId="1">Sheet2!$A$1:$B$1707</definedName>
   </definedNames>
   <calcPr calcId="179021" concurrentCalc="0"/>
@@ -21,9 +21,6 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3856" uniqueCount="3282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="3282">
   <si>
     <t>City</t>
   </si>
@@ -9969,7 +9966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -10001,6 +9998,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10311,8 +10309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10369,6 +10367,9 @@
       <c r="F2" s="5">
         <v>2298</v>
       </c>
+      <c r="G2">
+        <v>38217</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -10390,6 +10391,9 @@
       <c r="F3" s="5">
         <v>1140</v>
       </c>
+      <c r="G3">
+        <v>24925</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -10411,6 +10415,9 @@
       <c r="F4" s="5">
         <v>1191</v>
       </c>
+      <c r="G4">
+        <v>22814</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -10432,6 +10439,9 @@
       <c r="F5" s="5">
         <v>2378</v>
       </c>
+      <c r="G5">
+        <v>25785</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
@@ -10452,6 +10462,9 @@
       </c>
       <c r="F6" s="5">
         <v>1186</v>
+      </c>
+      <c r="G6">
+        <v>18116</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="8"/>
@@ -10479,6 +10492,9 @@
       <c r="F7" s="5">
         <v>1172</v>
       </c>
+      <c r="G7">
+        <v>17002</v>
+      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="9"/>
       <c r="M7" s="2"/>
@@ -10505,6 +10521,9 @@
       <c r="F8" s="5">
         <v>2127</v>
       </c>
+      <c r="G8">
+        <v>19001</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -10526,6 +10545,9 @@
       <c r="F9" s="5">
         <v>1100</v>
       </c>
+      <c r="G9">
+        <v>13020</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -10547,6 +10569,9 @@
       <c r="F10" s="5">
         <v>1070</v>
       </c>
+      <c r="G10">
+        <v>12955</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -10568,6 +10593,9 @@
       <c r="F11" s="5">
         <v>2281</v>
       </c>
+      <c r="G11">
+        <v>22281</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -10589,6 +10617,9 @@
       <c r="F12" s="5">
         <v>1185</v>
       </c>
+      <c r="G12">
+        <v>17114</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
@@ -10610,6 +10641,9 @@
       <c r="F13" s="5">
         <v>1044</v>
       </c>
+      <c r="G13">
+        <v>11170</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -10631,6 +10665,9 @@
       <c r="F14" s="5">
         <v>2089</v>
       </c>
+      <c r="G14">
+        <v>13726</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
@@ -10652,6 +10689,9 @@
       <c r="F15" s="5">
         <v>1033</v>
       </c>
+      <c r="G15">
+        <v>7609</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
@@ -10673,8 +10713,11 @@
       <c r="F16" s="5">
         <v>994</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>8084</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>6</v>
       </c>
@@ -10694,8 +10737,11 @@
       <c r="F17" s="5">
         <v>2019</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>20283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>6</v>
       </c>
@@ -10715,8 +10761,11 @@
       <c r="F18" s="5">
         <v>994</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>11899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
@@ -10736,8 +10785,11 @@
       <c r="F19" s="5">
         <v>948</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>10455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>7</v>
       </c>
@@ -10757,8 +10809,17 @@
       <c r="F20" s="5">
         <v>8276</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>151881</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>7</v>
       </c>
@@ -10778,8 +10839,17 @@
       <c r="F21" s="5">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>2332</v>
+      </c>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>7</v>
       </c>
@@ -10799,8 +10869,17 @@
       <c r="F22" s="5">
         <v>236</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>4815</v>
+      </c>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>7</v>
       </c>
@@ -10820,8 +10899,11 @@
       <c r="F23" s="5">
         <v>8400</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>96007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>7</v>
       </c>
@@ -10841,8 +10923,11 @@
       <c r="F24" s="5">
         <v>174</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>7</v>
       </c>
@@ -10862,8 +10947,11 @@
       <c r="F25" s="5">
         <v>242</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>3329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>7</v>
       </c>
@@ -10883,8 +10971,11 @@
       <c r="F26" s="5">
         <v>8065</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>54854</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>7</v>
       </c>
@@ -10904,8 +10995,11 @@
       <c r="F27" s="5">
         <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>7</v>
       </c>
@@ -10925,8 +11019,11 @@
       <c r="F28" s="5">
         <v>232</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>7</v>
       </c>
@@ -10946,8 +11043,11 @@
       <c r="F29" s="5">
         <v>8349</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>68643</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>7</v>
       </c>
@@ -10967,8 +11067,11 @@
       <c r="F30" s="5">
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>7</v>
       </c>
@@ -10988,8 +11091,11 @@
       <c r="F31" s="5">
         <v>238</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>7</v>
       </c>
@@ -11009,8 +11115,11 @@
       <c r="F32" s="5">
         <v>7729</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>39659</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>7</v>
       </c>
@@ -11030,8 +11139,11 @@
       <c r="F33" s="5">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>7</v>
       </c>
@@ -11051,8 +11163,11 @@
       <c r="F34" s="5">
         <v>231</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>7</v>
       </c>
@@ -11072,8 +11187,11 @@
       <c r="F35" s="5">
         <v>7849</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>63382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>7</v>
       </c>
@@ -11093,8 +11211,11 @@
       <c r="F36" s="5">
         <v>103</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>7</v>
       </c>
@@ -11114,8 +11235,11 @@
       <c r="F37" s="5">
         <v>231</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>8</v>
       </c>
@@ -11135,8 +11259,11 @@
       <c r="F38" s="5">
         <v>5766</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>125296</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>8</v>
       </c>
@@ -11156,8 +11283,11 @@
       <c r="F39" s="5">
         <v>7015</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>158859</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>8</v>
       </c>
@@ -11177,8 +11307,11 @@
       <c r="F40" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>8</v>
       </c>
@@ -11198,8 +11331,11 @@
       <c r="F41" s="5">
         <v>5881</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>83869</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>8</v>
       </c>
@@ -11219,8 +11355,11 @@
       <c r="F42" s="5">
         <v>7160</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>104779</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>8</v>
       </c>
@@ -11240,8 +11379,11 @@
       <c r="F43" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>8</v>
       </c>
@@ -11261,8 +11403,11 @@
       <c r="F44" s="5">
         <v>5469</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>50504</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>8</v>
       </c>
@@ -11282,8 +11427,11 @@
       <c r="F45" s="5">
         <v>6916</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>51379</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>8</v>
       </c>
@@ -11303,8 +11451,11 @@
       <c r="F46" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>8</v>
       </c>
@@ -11324,8 +11475,11 @@
       <c r="F47" s="5">
         <v>5596</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>53374</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>8</v>
       </c>
@@ -11345,8 +11499,11 @@
       <c r="F48" s="5">
         <v>6968</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>64220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>8</v>
       </c>
@@ -11366,8 +11523,11 @@
       <c r="F49" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>8</v>
       </c>
@@ -11387,8 +11547,11 @@
       <c r="F50" s="5">
         <v>5051</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>37728</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>8</v>
       </c>
@@ -11408,8 +11571,11 @@
       <c r="F51" s="5">
         <v>5824</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>40116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>8</v>
       </c>
@@ -11429,8 +11595,11 @@
       <c r="F52" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>8</v>
       </c>
@@ -11450,8 +11619,11 @@
       <c r="F53" s="5">
         <v>5399</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>71932</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>8</v>
       </c>
@@ -11471,8 +11643,11 @@
       <c r="F54" s="5">
         <v>5640</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>64947</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>8</v>
       </c>
@@ -11492,8 +11667,11 @@
       <c r="F55" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>9</v>
       </c>
@@ -11513,8 +11691,11 @@
       <c r="F56" s="5">
         <v>3651</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>60020</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>9</v>
       </c>
@@ -11534,8 +11715,11 @@
       <c r="F57" s="5">
         <v>2495</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>24223</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>9</v>
       </c>
@@ -11555,8 +11739,11 @@
       <c r="F58" s="5">
         <v>3635</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>57133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>9</v>
       </c>
@@ -11576,8 +11763,11 @@
       <c r="F59" s="5">
         <v>3565</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>46957</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>9</v>
       </c>
@@ -11597,8 +11787,11 @@
       <c r="F60" s="5">
         <v>2574</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>25341</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>9</v>
       </c>
@@ -11618,8 +11811,11 @@
       <c r="F61" s="5">
         <v>3710</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>79989</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>9</v>
       </c>
@@ -11639,8 +11835,11 @@
       <c r="F62" s="5">
         <v>3037</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>21951</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>9</v>
       </c>
@@ -11660,8 +11859,11 @@
       <c r="F63" s="5">
         <v>2184</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>11876</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>9</v>
       </c>
@@ -11681,8 +11883,11 @@
       <c r="F64" s="5">
         <v>3443</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>40984</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>9</v>
       </c>
@@ -11702,8 +11907,11 @@
       <c r="F65" s="5">
         <v>3169</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>28001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>9</v>
       </c>
@@ -11723,8 +11931,11 @@
       <c r="F66" s="5">
         <v>2306</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>21024</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>9</v>
       </c>
@@ -11744,8 +11955,11 @@
       <c r="F67" s="5">
         <v>3644</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>47446</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>9</v>
       </c>
@@ -11765,8 +11979,11 @@
       <c r="F68" s="5">
         <v>2936</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>28347</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>9</v>
       </c>
@@ -11786,8 +12003,11 @@
       <c r="F69" s="5">
         <v>2197</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>14737</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>9</v>
       </c>
@@ -11807,8 +12027,11 @@
       <c r="F70" s="5">
         <v>3495</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>36585</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>9</v>
       </c>
@@ -11828,8 +12051,11 @@
       <c r="F71" s="5">
         <v>3246</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>39717</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>9</v>
       </c>
@@ -11849,8 +12075,11 @@
       <c r="F72" s="5">
         <v>2358</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>16199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>9</v>
       </c>
@@ -11870,8 +12099,11 @@
       <c r="F73" s="5">
         <v>3431</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>33927</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>17</v>
       </c>
@@ -11891,8 +12123,11 @@
       <c r="F74" s="5">
         <v>1862</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>28003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>17</v>
       </c>
@@ -11912,8 +12147,11 @@
       <c r="F75" s="5">
         <v>745</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>16373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>17</v>
       </c>
@@ -11933,8 +12171,11 @@
       <c r="F76" s="5">
         <v>957</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>19264</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>17</v>
       </c>
@@ -11954,8 +12195,11 @@
       <c r="F77" s="5">
         <v>1949</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>24952</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>17</v>
       </c>
@@ -11975,8 +12219,11 @@
       <c r="F78" s="5">
         <v>788</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>16298</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>17</v>
       </c>
@@ -11996,8 +12243,11 @@
       <c r="F79" s="5">
         <v>949</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>14811</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>17</v>
       </c>
@@ -12017,8 +12267,11 @@
       <c r="F80" s="5">
         <v>1866</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <v>12864</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>17</v>
       </c>
@@ -12038,8 +12291,11 @@
       <c r="F81" s="5">
         <v>772</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>17</v>
       </c>
@@ -12059,8 +12315,11 @@
       <c r="F82" s="5">
         <v>899</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <v>7861</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>17</v>
       </c>
@@ -12080,8 +12339,11 @@
       <c r="F83" s="5">
         <v>2033</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <v>18877</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>17</v>
       </c>
@@ -12101,8 +12363,11 @@
       <c r="F84" s="5">
         <v>837</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <v>10661</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>17</v>
       </c>
@@ -12122,8 +12387,11 @@
       <c r="F85" s="5">
         <v>936</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <v>10475</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>17</v>
       </c>
@@ -12143,8 +12411,11 @@
       <c r="F86" s="5">
         <v>1767</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <v>9622</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>17</v>
       </c>
@@ -12164,8 +12435,11 @@
       <c r="F87" s="5">
         <v>770</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>17</v>
       </c>
@@ -12185,8 +12459,11 @@
       <c r="F88" s="5">
         <v>910</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <v>10408</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>17</v>
       </c>
@@ -12206,8 +12483,11 @@
       <c r="F89" s="5">
         <v>1733</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <v>26367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>17</v>
       </c>
@@ -12227,8 +12507,11 @@
       <c r="F90" s="5">
         <v>736</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <v>6871</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>17</v>
       </c>
@@ -12248,8 +12531,11 @@
       <c r="F91" s="5">
         <v>927</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <v>18618</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>18</v>
       </c>
@@ -12269,8 +12555,11 @@
       <c r="F92" s="5">
         <v>669</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <v>13382</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>18</v>
       </c>
@@ -12290,8 +12579,11 @@
       <c r="F93" s="5">
         <v>4647</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <v>110983</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>18</v>
       </c>
@@ -12311,8 +12603,11 @@
       <c r="F94" s="5">
         <v>634</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <v>17915</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>18</v>
       </c>
@@ -12332,8 +12627,11 @@
       <c r="F95" s="5">
         <v>695</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <v>8544</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>18</v>
       </c>
@@ -12353,8 +12651,11 @@
       <c r="F96" s="5">
         <v>4775</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <v>90257</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>18</v>
       </c>
@@ -12374,8 +12675,11 @@
       <c r="F97" s="5">
         <v>609</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97">
+        <v>12841</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>18</v>
       </c>
@@ -12395,8 +12699,11 @@
       <c r="F98" s="5">
         <v>609</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>18</v>
       </c>
@@ -12416,8 +12723,11 @@
       <c r="F99" s="5">
         <v>4317</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99">
+        <v>48659</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>18</v>
       </c>
@@ -12437,8 +12747,11 @@
       <c r="F100" s="5">
         <v>499</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100">
+        <v>8746</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>18</v>
       </c>
@@ -12458,8 +12771,11 @@
       <c r="F101" s="5">
         <v>640</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101">
+        <v>4303</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>18</v>
       </c>
@@ -12479,8 +12795,11 @@
       <c r="F102" s="5">
         <v>4654</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102">
+        <v>52934</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>18</v>
       </c>
@@ -12500,8 +12819,11 @@
       <c r="F103" s="5">
         <v>545</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103">
+        <v>6201</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>18</v>
       </c>
@@ -12521,8 +12843,11 @@
       <c r="F104" s="5">
         <v>592</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104">
+        <v>4642</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>18</v>
       </c>
@@ -12542,8 +12867,11 @@
       <c r="F105" s="5">
         <v>4622</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105">
+        <v>51907</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>18</v>
       </c>
@@ -12563,8 +12891,11 @@
       <c r="F106" s="5">
         <v>541</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106">
+        <v>8629</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>18</v>
       </c>
@@ -12584,8 +12915,11 @@
       <c r="F107" s="5">
         <v>676</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107">
+        <v>7507</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>18</v>
       </c>
@@ -12605,8 +12939,11 @@
       <c r="F108" s="5">
         <v>4772</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108">
+        <v>69055</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>18</v>
       </c>
@@ -12626,8 +12963,11 @@
       <c r="F109" s="5">
         <v>530</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109">
+        <v>11418</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>19</v>
       </c>
@@ -12647,8 +12987,11 @@
       <c r="F110" s="5">
         <v>978</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110">
+        <v>10223</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>19</v>
       </c>
@@ -12668,8 +13011,11 @@
       <c r="F111" s="5">
         <v>990</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111">
+        <v>7787</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>19</v>
       </c>
@@ -12689,8 +13035,11 @@
       <c r="F112" s="5">
         <v>1263</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112">
+        <v>13842</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>19</v>
       </c>
@@ -12710,8 +13059,11 @@
       <c r="F113" s="5">
         <v>951</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113">
+        <v>8219</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>19</v>
       </c>
@@ -12731,8 +13083,11 @@
       <c r="F114" s="5">
         <v>1068</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114">
+        <v>15018</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>19</v>
       </c>
@@ -12752,8 +13107,11 @@
       <c r="F115" s="5">
         <v>1298</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115">
+        <v>21401</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>19</v>
       </c>
@@ -12773,8 +13131,11 @@
       <c r="F116" s="5">
         <v>762</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>19</v>
       </c>
@@ -12794,8 +13155,11 @@
       <c r="F117" s="5">
         <v>894</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>19</v>
       </c>
@@ -12815,8 +13179,11 @@
       <c r="F118" s="5">
         <v>1065</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118">
+        <v>10504</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>19</v>
       </c>
@@ -12836,8 +13203,11 @@
       <c r="F119" s="5">
         <v>733</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119">
+        <v>5518</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>19</v>
       </c>
@@ -12857,8 +13227,11 @@
       <c r="F120" s="5">
         <v>892</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120">
+        <v>9497</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
         <v>19</v>
       </c>
@@ -12878,8 +13251,11 @@
       <c r="F121" s="5">
         <v>1041</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121">
+        <v>9656</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
         <v>19</v>
       </c>
@@ -12899,8 +13275,11 @@
       <c r="F122" s="5">
         <v>621</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122">
+        <v>9349</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>19</v>
       </c>
@@ -12920,8 +13299,11 @@
       <c r="F123" s="5">
         <v>826</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123">
+        <v>10194</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>19</v>
       </c>
@@ -12941,8 +13323,11 @@
       <c r="F124" s="5">
         <v>994</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124">
+        <v>11820</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>19</v>
       </c>
@@ -12962,8 +13347,11 @@
       <c r="F125" s="5">
         <v>713</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125">
+        <v>6714</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
         <v>19</v>
       </c>
@@ -12983,8 +13371,11 @@
       <c r="F126" s="5">
         <v>833</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126">
+        <v>7560</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
         <v>19</v>
       </c>
@@ -13004,8 +13395,11 @@
       <c r="F127" s="5">
         <v>965</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127">
+        <v>13616</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>20</v>
       </c>
@@ -13025,8 +13419,11 @@
       <c r="F128" s="5">
         <v>2163</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128">
+        <v>39012</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>20</v>
       </c>
@@ -13046,8 +13443,11 @@
       <c r="F129" s="5">
         <v>417</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129">
+        <v>7459</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>20</v>
       </c>
@@ -13067,8 +13467,11 @@
       <c r="F130" s="5">
         <v>1282</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130">
+        <v>21232</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>20</v>
       </c>
@@ -13088,8 +13491,11 @@
       <c r="F131" s="5">
         <v>2222</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131">
+        <v>27035</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>20</v>
       </c>
@@ -13109,8 +13515,11 @@
       <c r="F132" s="5">
         <v>464</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132">
+        <v>4359</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>20</v>
       </c>
@@ -13130,8 +13539,11 @@
       <c r="F133" s="5">
         <v>1286</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133">
+        <v>16905</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>20</v>
       </c>
@@ -13151,8 +13563,11 @@
       <c r="F134" s="5">
         <v>2040</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134">
+        <v>16647</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
         <v>20</v>
       </c>
@@ -13172,8 +13587,11 @@
       <c r="F135" s="5">
         <v>450</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135">
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>20</v>
       </c>
@@ -13193,8 +13611,11 @@
       <c r="F136" s="5">
         <v>1240</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136">
+        <v>11698</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
         <v>20</v>
       </c>
@@ -13214,8 +13635,11 @@
       <c r="F137" s="5">
         <v>2050</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137">
+        <v>14764</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
         <v>20</v>
       </c>
@@ -13235,8 +13659,11 @@
       <c r="F138" s="5">
         <v>490</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>20</v>
       </c>
@@ -13256,8 +13683,11 @@
       <c r="F139" s="5">
         <v>1286</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139">
+        <v>13712</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
         <v>20</v>
       </c>
@@ -13277,8 +13707,11 @@
       <c r="F140" s="5">
         <v>1919</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140">
+        <v>14459</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>20</v>
       </c>
@@ -13298,8 +13731,11 @@
       <c r="F141" s="5">
         <v>499</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
         <v>20</v>
       </c>
@@ -13319,8 +13755,11 @@
       <c r="F142" s="5">
         <v>1227</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142">
+        <v>12025</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>20</v>
       </c>
@@ -13340,8 +13779,11 @@
       <c r="F143" s="5">
         <v>1909</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143">
+        <v>18268</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>20</v>
       </c>
@@ -13361,8 +13803,11 @@
       <c r="F144" s="5">
         <v>403</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>20</v>
       </c>
@@ -13382,8 +13827,13 @@
       <c r="F145" s="5">
         <v>1265</v>
       </c>
+      <c r="G145">
+        <v>14080</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G145" xr:uid="{86AD0A80-12C8-4902-A4F7-E008F189B3E5}"/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>